<commit_message>
add sims for pre99 and measureb
</commit_message>
<xml_diff>
--- a/inputs/data_raw/Data_SJPF_Demographics_20190630.xlsx
+++ b/inputs/data_raw/Data_SJPF_Demographics_20190630.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Proj_CAPlans\model_SJ\inputs\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCFCF32-C0BC-439C-9022-7656A0EEE0FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E98A17-553B-498C-9761-14762BDE8166}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1845" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="other" sheetId="37" r:id="rId1"/>
@@ -1092,9 +1092,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1118,6 +1115,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1928,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF5E2A8-8066-4C09-9596-AB1EEC0396D2}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3391,10 +3391,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F86E88DF-A66D-4D5B-9543-81B9EF75DDB4}">
-  <dimension ref="A2:J32"/>
+  <dimension ref="A2:J34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:I31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3418,10 +3418,10 @@
       <c r="D4" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="72"/>
+      <c r="F4" s="71"/>
       <c r="G4" s="44" t="s">
         <v>89</v>
       </c>
@@ -3798,10 +3798,10 @@
       <c r="D20" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="73" t="s">
+      <c r="E20" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="F20" s="73"/>
+      <c r="F20" s="72"/>
       <c r="G20" s="62" t="s">
         <v>97</v>
       </c>
@@ -3816,317 +3816,317 @@
       </c>
     </row>
     <row r="21" spans="2:10">
-      <c r="B21" s="66">
+      <c r="B21" s="65">
         <v>103799</v>
       </c>
-      <c r="C21" s="66">
+      <c r="C21" s="65">
         <v>110446</v>
       </c>
-      <c r="D21" s="66">
-        <v>0</v>
-      </c>
-      <c r="E21" s="66">
-        <v>0</v>
-      </c>
-      <c r="F21" s="66">
-        <v>0</v>
-      </c>
-      <c r="G21" s="66">
-        <v>0</v>
-      </c>
-      <c r="H21" s="66">
-        <v>0</v>
-      </c>
-      <c r="I21" s="66">
-        <v>0</v>
-      </c>
-      <c r="J21" s="67" t="s">
+      <c r="D21" s="65">
+        <v>0</v>
+      </c>
+      <c r="E21" s="65">
+        <v>0</v>
+      </c>
+      <c r="F21" s="65">
+        <v>0</v>
+      </c>
+      <c r="G21" s="65">
+        <v>0</v>
+      </c>
+      <c r="H21" s="65">
+        <v>0</v>
+      </c>
+      <c r="I21" s="65">
+        <v>0</v>
+      </c>
+      <c r="J21" s="66" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="22" spans="2:10">
-      <c r="B22" s="66">
+      <c r="B22" s="65">
         <v>102715</v>
       </c>
-      <c r="C22" s="66">
+      <c r="C22" s="65">
         <v>113854</v>
       </c>
-      <c r="D22" s="66">
+      <c r="D22" s="65">
         <v>137451</v>
       </c>
-      <c r="E22" s="66">
-        <v>0</v>
-      </c>
-      <c r="F22" s="66">
-        <v>0</v>
-      </c>
-      <c r="G22" s="66">
-        <v>0</v>
-      </c>
-      <c r="H22" s="66">
-        <v>0</v>
-      </c>
-      <c r="I22" s="66">
-        <v>0</v>
-      </c>
-      <c r="J22" s="67">
+      <c r="E22" s="65">
+        <v>0</v>
+      </c>
+      <c r="F22" s="65">
+        <v>0</v>
+      </c>
+      <c r="G22" s="65">
+        <v>0</v>
+      </c>
+      <c r="H22" s="65">
+        <v>0</v>
+      </c>
+      <c r="I22" s="65">
+        <v>0</v>
+      </c>
+      <c r="J22" s="66">
         <v>110734</v>
       </c>
     </row>
     <row r="23" spans="2:10">
-      <c r="B23" s="66">
+      <c r="B23" s="65">
         <v>104131</v>
       </c>
-      <c r="C23" s="66">
+      <c r="C23" s="65">
         <v>115691</v>
       </c>
-      <c r="D23" s="66">
+      <c r="D23" s="65">
         <v>138932</v>
       </c>
-      <c r="E23" s="66">
+      <c r="E23" s="65">
         <v>140531</v>
       </c>
-      <c r="F23" s="66">
-        <v>0</v>
-      </c>
-      <c r="G23" s="66">
-        <v>0</v>
-      </c>
-      <c r="H23" s="66">
-        <v>0</v>
-      </c>
-      <c r="I23" s="66">
-        <v>0</v>
-      </c>
-      <c r="J23" s="67">
+      <c r="F23" s="65">
+        <v>0</v>
+      </c>
+      <c r="G23" s="65">
+        <v>0</v>
+      </c>
+      <c r="H23" s="65">
+        <v>0</v>
+      </c>
+      <c r="I23" s="65">
+        <v>0</v>
+      </c>
+      <c r="J23" s="66">
         <v>120758</v>
       </c>
     </row>
     <row r="24" spans="2:10">
-      <c r="B24" s="66">
+      <c r="B24" s="65">
         <v>101048</v>
       </c>
-      <c r="C24" s="66">
+      <c r="C24" s="65">
         <v>118417</v>
       </c>
-      <c r="D24" s="66">
+      <c r="D24" s="65">
         <v>136831</v>
       </c>
-      <c r="E24" s="66">
+      <c r="E24" s="65">
         <v>145149</v>
       </c>
-      <c r="F24" s="66">
+      <c r="F24" s="65">
         <v>160194</v>
       </c>
-      <c r="G24" s="66">
-        <v>0</v>
-      </c>
-      <c r="H24" s="66">
-        <v>0</v>
-      </c>
-      <c r="I24" s="66">
-        <v>0</v>
-      </c>
-      <c r="J24" s="67">
+      <c r="G24" s="65">
+        <v>0</v>
+      </c>
+      <c r="H24" s="65">
+        <v>0</v>
+      </c>
+      <c r="I24" s="65">
+        <v>0</v>
+      </c>
+      <c r="J24" s="66">
         <v>134964</v>
       </c>
     </row>
     <row r="25" spans="2:10">
-      <c r="B25" s="66">
+      <c r="B25" s="65">
         <v>92443</v>
       </c>
-      <c r="C25" s="66">
+      <c r="C25" s="65">
         <v>116496</v>
       </c>
-      <c r="D25" s="66">
+      <c r="D25" s="65">
         <v>135855</v>
       </c>
-      <c r="E25" s="66">
+      <c r="E25" s="65">
         <v>141636</v>
       </c>
-      <c r="F25" s="66">
+      <c r="F25" s="65">
         <v>153916</v>
       </c>
-      <c r="G25" s="66">
+      <c r="G25" s="65">
         <v>165105</v>
       </c>
-      <c r="H25" s="66">
-        <v>0</v>
-      </c>
-      <c r="I25" s="66">
-        <v>0</v>
-      </c>
-      <c r="J25" s="67">
+      <c r="H25" s="65">
+        <v>0</v>
+      </c>
+      <c r="I25" s="65">
+        <v>0</v>
+      </c>
+      <c r="J25" s="66">
         <v>142691</v>
       </c>
     </row>
     <row r="26" spans="2:10">
-      <c r="B26" s="66">
+      <c r="B26" s="65">
         <v>112910</v>
       </c>
-      <c r="C26" s="66">
+      <c r="C26" s="65">
         <v>128424</v>
       </c>
-      <c r="D26" s="66">
+      <c r="D26" s="65">
         <v>136011</v>
       </c>
-      <c r="E26" s="66">
+      <c r="E26" s="65">
         <v>139860</v>
       </c>
-      <c r="F26" s="66">
+      <c r="F26" s="65">
         <v>146572</v>
       </c>
-      <c r="G26" s="66">
+      <c r="G26" s="65">
         <v>158569</v>
       </c>
-      <c r="H26" s="66">
+      <c r="H26" s="65">
         <v>191598</v>
       </c>
-      <c r="I26" s="66">
-        <v>0</v>
-      </c>
-      <c r="J26" s="67">
+      <c r="I26" s="65">
+        <v>0</v>
+      </c>
+      <c r="J26" s="66">
         <v>151470</v>
       </c>
     </row>
     <row r="27" spans="2:10">
-      <c r="B27" s="66">
+      <c r="B27" s="65">
         <v>151735</v>
       </c>
-      <c r="C27" s="66">
+      <c r="C27" s="65">
         <v>108969</v>
       </c>
-      <c r="D27" s="66">
+      <c r="D27" s="65">
         <v>124207</v>
       </c>
-      <c r="E27" s="66">
+      <c r="E27" s="65">
         <v>143466</v>
       </c>
-      <c r="F27" s="66">
+      <c r="F27" s="65">
         <v>146610</v>
       </c>
-      <c r="G27" s="66">
+      <c r="G27" s="65">
         <v>156402</v>
       </c>
-      <c r="H27" s="66">
+      <c r="H27" s="65">
         <v>169465</v>
       </c>
-      <c r="I27" s="66">
+      <c r="I27" s="65">
         <v>172483</v>
       </c>
-      <c r="J27" s="67">
+      <c r="J27" s="66">
         <v>155344</v>
       </c>
     </row>
     <row r="28" spans="2:10">
-      <c r="B28" s="66">
-        <v>0</v>
-      </c>
-      <c r="C28" s="66">
+      <c r="B28" s="65">
+        <v>0</v>
+      </c>
+      <c r="C28" s="65">
         <v>127830</v>
       </c>
-      <c r="D28" s="66">
+      <c r="D28" s="65">
         <v>121337</v>
       </c>
-      <c r="E28" s="66">
+      <c r="E28" s="65">
         <v>158923</v>
       </c>
-      <c r="F28" s="66">
+      <c r="F28" s="65">
         <v>141086</v>
       </c>
-      <c r="G28" s="66">
+      <c r="G28" s="65">
         <v>149699</v>
       </c>
-      <c r="H28" s="66">
+      <c r="H28" s="65">
         <v>149547</v>
       </c>
-      <c r="I28" s="66">
+      <c r="I28" s="65">
         <v>147326</v>
       </c>
-      <c r="J28" s="67">
+      <c r="J28" s="66">
         <v>147193</v>
       </c>
     </row>
     <row r="29" spans="2:10">
-      <c r="B29" s="66">
-        <v>0</v>
-      </c>
-      <c r="C29" s="66">
-        <v>0</v>
-      </c>
-      <c r="D29" s="66">
-        <v>0</v>
-      </c>
-      <c r="E29" s="66">
-        <v>0</v>
-      </c>
-      <c r="F29" s="66">
+      <c r="B29" s="65">
+        <v>0</v>
+      </c>
+      <c r="C29" s="65">
+        <v>0</v>
+      </c>
+      <c r="D29" s="65">
+        <v>0</v>
+      </c>
+      <c r="E29" s="65">
+        <v>0</v>
+      </c>
+      <c r="F29" s="65">
         <v>133961</v>
       </c>
-      <c r="G29" s="66">
+      <c r="G29" s="65">
         <v>150624</v>
       </c>
-      <c r="H29" s="66">
+      <c r="H29" s="65">
         <v>170519</v>
       </c>
-      <c r="I29" s="66">
-        <v>0</v>
-      </c>
-      <c r="J29" s="67">
+      <c r="I29" s="65">
+        <v>0</v>
+      </c>
+      <c r="J29" s="66">
         <v>145608</v>
       </c>
     </row>
     <row r="30" spans="2:10">
-      <c r="B30" s="66">
-        <v>0</v>
-      </c>
-      <c r="C30" s="66">
-        <v>0</v>
-      </c>
-      <c r="D30" s="66">
-        <v>0</v>
-      </c>
-      <c r="E30" s="66">
-        <v>0</v>
-      </c>
-      <c r="F30" s="66">
-        <v>0</v>
-      </c>
-      <c r="G30" s="66">
-        <v>0</v>
-      </c>
-      <c r="H30" s="66">
-        <v>0</v>
-      </c>
-      <c r="I30" s="66">
-        <v>0</v>
-      </c>
-      <c r="J30" s="67">
+      <c r="B30" s="65">
+        <v>0</v>
+      </c>
+      <c r="C30" s="65">
+        <v>0</v>
+      </c>
+      <c r="D30" s="65">
+        <v>0</v>
+      </c>
+      <c r="E30" s="65">
+        <v>0</v>
+      </c>
+      <c r="F30" s="65">
+        <v>0</v>
+      </c>
+      <c r="G30" s="65">
+        <v>0</v>
+      </c>
+      <c r="H30" s="65">
+        <v>0</v>
+      </c>
+      <c r="I30" s="65">
+        <v>0</v>
+      </c>
+      <c r="J30" s="66">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B31" s="68">
-        <v>0</v>
-      </c>
-      <c r="C31" s="68">
-        <v>0</v>
-      </c>
-      <c r="D31" s="68">
-        <v>0</v>
-      </c>
-      <c r="E31" s="68">
-        <v>0</v>
-      </c>
-      <c r="F31" s="68">
-        <v>0</v>
-      </c>
-      <c r="G31" s="68">
-        <v>0</v>
-      </c>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
-      <c r="J31" s="70">
+      <c r="B31" s="67">
+        <v>0</v>
+      </c>
+      <c r="C31" s="67">
+        <v>0</v>
+      </c>
+      <c r="D31" s="67">
+        <v>0</v>
+      </c>
+      <c r="E31" s="67">
+        <v>0</v>
+      </c>
+      <c r="F31" s="67">
+        <v>0</v>
+      </c>
+      <c r="G31" s="67">
+        <v>0</v>
+      </c>
+      <c r="H31" s="68"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="69">
         <v>0</v>
       </c>
     </row>
@@ -4155,8 +4155,14 @@
       <c r="I32" s="64" t="s">
         <v>106</v>
       </c>
-      <c r="J32" s="65" t="s">
+      <c r="J32" s="73" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="10:10">
+      <c r="J34" s="40">
+        <f>J16*J32</f>
+        <v>235818135</v>
       </c>
     </row>
   </sheetData>
@@ -4215,7 +4221,7 @@
       <c r="D7" s="34">
         <v>92</v>
       </c>
-      <c r="E7" s="71">
+      <c r="E7" s="70">
         <v>4836737</v>
       </c>
     </row>

</xml_diff>